<commit_message>
Modellen med ny kalibreringsprocedure kører!!!
tilføjet nnnn+ i nesting_tree, nesting_trees. Kataloget "new2" kører.
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/techdata_new2.xlsx
+++ b/examples/Abatement/Data/techdata_new2.xlsx
@@ -1353,8 +1353,8 @@
   <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M5" sqref="M5"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,10 +1476,10 @@
         <v>0.25</v>
       </c>
       <c r="K2">
-        <v>0.09</v>
+        <v>0.04</v>
       </c>
       <c r="M2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T2">
         <v>0.5</v>
@@ -1505,13 +1505,13 @@
         <v>0.25</v>
       </c>
       <c r="J3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="K3">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="M3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T3">
         <v>0.5</v>
@@ -1540,7 +1540,7 @@
         <v>0.1</v>
       </c>
       <c r="M4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -1557,7 +1557,7 @@
         <v>0.05</v>
       </c>
       <c r="M5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z5">
         <v>0.5</v>
@@ -1580,7 +1580,7 @@
         <v>0.05</v>
       </c>
       <c r="M6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z6">
         <v>0.5</v>

</xml_diff>